<commit_message>
update mysql.conf slow-query, nginx.conf 504-timeout; add importable files.
</commit_message>
<xml_diff>
--- a/test/模板_卷详目.xlsx
+++ b/test/模板_卷详目.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600"/>
+    <workbookView xWindow="-28540" yWindow="4880" windowWidth="24680" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -894,6 +894,12 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -993,7 +999,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="145">
     <cellStyle name="20% - 强调文字颜色 1 2" xfId="1"/>
     <cellStyle name="20% - 强调文字颜色 2 2" xfId="18"/>
     <cellStyle name="20% - 强调文字颜色 3 2" xfId="20"/>
@@ -1080,6 +1086,9 @@
     <cellStyle name="超链接" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
@@ -1109,6 +1118,9 @@
     <cellStyle name="访问过的超链接" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="好 2" xfId="67"/>
     <cellStyle name="汇总 2" xfId="68"/>
     <cellStyle name="计算 2" xfId="3"/>
@@ -1431,11 +1443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1797,6 +1809,69 @@
         <v>37</v>
       </c>
       <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="3:9">
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="3:9">
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="3:9">
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="27" type="noConversion"/>

</xml_diff>